<commit_message>
fix : update test data
</commit_message>
<xml_diff>
--- a/zoho-crm-integration-suite/testData/testdata.xlsx
+++ b/zoho-crm-integration-suite/testData/testdata.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prajjawalmodi/Downloads/zoho-crm-integration-suite/testData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE00615C-8669-5B46-B704-3549CFC1261B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{A96DF1A6-E73E-334D-8622-DC6AA642AEE5}"/>
+    <workbookView xWindow="1500" yWindow="1320" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login-Credentials" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
     <sheet name="Delete-Lead" sheetId="5" r:id="rId5"/>
     <sheet name="Customize-Lead" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="66">
   <si>
     <t>password</t>
   </si>
@@ -229,22 +223,22 @@
     <t>Lead Image</t>
   </si>
   <si>
-    <t>prajjawalmodi05@gmail.com</t>
-  </si>
-  <si>
-    <t>Password@1313</t>
-  </si>
-  <si>
     <t>Password@9191</t>
   </si>
   <si>
     <t>1121-2331</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>Shinchain@1100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -361,7 +355,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -413,7 +407,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -627,25 +621,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792A2689-677C-9B4E-8A83-B810A5E1E3BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.1640625" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="4" width="78" customWidth="1"/>
   </cols>
   <sheetData>
@@ -663,26 +657,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17">
+    <row r="2" spans="1:4" ht="16.5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17">
+    <row r="3" spans="1:4" ht="16.5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -695,8 +692,8 @@
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>910191</v>
+      <c r="C4" t="s">
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -706,11 +703,17 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
+    <row r="6" spans="1:4" ht="16.5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -721,15 +724,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17">
+    <row r="7" spans="1:4" ht="16.5">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -737,7 +740,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{ED01D078-2323-A645-BBB8-9BEB3B5BD265}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -745,22 +748,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D44532-40B0-0441-BF3E-FD84A915AE62}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="B2" sqref="B2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.83203125" customWidth="1"/>
+    <col min="1" max="1" width="42.77734375" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
+    <col min="9" max="9" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -792,15 +795,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17">
+    <row r="2" spans="1:9" ht="16.5">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>26</v>
@@ -821,15 +824,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17">
+    <row r="3" spans="1:9" ht="16.5">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -847,15 +850,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17">
+    <row r="4" spans="1:9" ht="16.5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -875,9 +878,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{314EBC44-59F0-9B4B-98AE-FD37C1F620D3}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{A5D9BA6F-C886-734E-B4FA-D48238D10401}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{8B70884B-9ADF-6D44-B1BB-FF8A619247DD}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -885,19 +888,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DFEB2F-12B2-BC4B-96C5-A8EF44A3FBB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="29.33203125" customWidth="1"/>
   </cols>
@@ -934,15 +937,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17">
+    <row r="2" spans="1:10" ht="16.5">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
@@ -954,18 +957,18 @@
         <v>21221121</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5">
       <c r="A3" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -980,18 +983,18 @@
         <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -1009,18 +1012,18 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5">
@@ -1031,14 +1034,14 @@
         <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{08710402-87E9-914E-8907-64F6EB9740F1}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{43E8A91A-59DA-4349-B8B4-FCB439CEEB3E}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{FEF4714A-74FE-4841-9E07-A88777901222}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1046,18 +1049,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5123A3-08FC-234B-BD47-C3BEA884B91E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
     <col min="7" max="7" width="25.6640625" customWidth="1"/>
   </cols>
@@ -1085,15 +1088,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17">
+    <row r="2" spans="1:7" ht="16.5">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>50</v>
@@ -1108,15 +1111,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17">
+    <row r="3" spans="1:7" ht="16.5">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>51</v>
@@ -1133,7 +1136,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{190EDDB0-E823-B846-948B-1C8C69ED6B57}"/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1141,19 +1144,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6BDD0C-49CB-2547-8EFA-78F35977B7DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1173,29 +1176,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17">
+    <row r="2" spans="1:5" ht="16.5">
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>62</v>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2">
         <v>21221121</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17">
+    <row r="3" spans="1:5" ht="16.5">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <v>21221121</v>
@@ -1206,7 +1209,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{FA39CD8D-88F5-C044-9B7D-A971C48BE4B8}"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1214,14 +1218,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7955F8-225D-1C40-8D2B-A2498BAE84C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -1246,7 +1250,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17">
+    <row r="2" spans="1:5" ht="16.5">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>58</v>
@@ -1263,7 +1267,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17">
+    <row r="3" spans="1:5" ht="16.5">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1271,7 +1275,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
@@ -1280,7 +1284,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17">
+    <row r="4" spans="1:5" ht="16.5">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1288,7 +1292,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>

</xml_diff>